<commit_message>
cambios en recibo + antiguedad reconocida empleado
</commit_message>
<xml_diff>
--- a/Woopin.SGC.Web/App_Data/Importaciones/Templates/Empleados.xlsx
+++ b/Woopin.SGC.Web/App_Data/Importaciones/Templates/Empleados.xlsx
@@ -11,6 +11,7 @@
     <sheet name="NOELIMINAR-Config" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Bancos_Depositos">'NOELIMINAR-Config'!$J$2:$J$5</definedName>
     <definedName name="Categorias">'NOELIMINAR-Config'!$F$2:$F$12</definedName>
     <definedName name="EstadoCivil">'NOELIMINAR-Config'!$D$2:$D$5</definedName>
     <definedName name="Localizaciones">'NOELIMINAR-Config'!$B$2:$B$21</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
   <si>
     <t>Dpto</t>
   </si>
@@ -343,6 +344,27 @@
   </si>
   <si>
     <t>O.S.De Relojeros Y Joyeros</t>
+  </si>
+  <si>
+    <t>Bancos Depositos</t>
+  </si>
+  <si>
+    <t>Banco Credicoop</t>
+  </si>
+  <si>
+    <t>Banco Galicia</t>
+  </si>
+  <si>
+    <t>Banco HSBC</t>
+  </si>
+  <si>
+    <t>Banco ICBC</t>
+  </si>
+  <si>
+    <t>Banco Deposito</t>
+  </si>
+  <si>
+    <t>Fecha Antiguedad Reconocida</t>
   </si>
 </sst>
 </file>
@@ -404,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -524,11 +546,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -560,6 +595,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W576"/>
+  <dimension ref="A1:Y576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -891,10 +927,12 @@
     <col min="21" max="21" width="11.54296875" style="1" customWidth="1"/>
     <col min="22" max="22" width="26" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.26953125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.90625" style="1"/>
+    <col min="24" max="24" width="15.36328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="26.54296875" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -964,8 +1002,14 @@
       <c r="W1" s="21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="str">
         <f>MID(A2,4,8)</f>
@@ -992,8 +1036,10 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="str">
         <f t="shared" ref="B3:B66" si="0">MID(A3,4,8)</f>
         <v/>
@@ -1003,7 +1049,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1013,7 +1059,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1023,7 +1069,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1033,7 +1079,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1043,7 +1089,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1053,7 +1099,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1063,7 +1109,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1073,7 +1119,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1083,7 +1129,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1093,7 +1139,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1103,7 +1149,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1113,7 +1159,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1123,7 +1169,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4425,7 +4471,7 @@
       <c r="F576" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F576">
       <formula1>Localizaciones</formula1>
     </dataValidation>
@@ -4450,6 +4496,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W142">
       <formula1>ObrasSociales</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X142">
+      <formula1>Bancos_Depositos</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4458,10 +4507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4474,11 +4523,12 @@
     <col min="6" max="6" width="27.08984375" style="6" customWidth="1"/>
     <col min="7" max="7" width="76.6328125" style="6" customWidth="1"/>
     <col min="8" max="8" width="26" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="11.54296875" style="6"/>
+    <col min="9" max="9" width="24.7265625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.90625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="11.54296875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
@@ -4503,8 +4553,11 @@
       <c r="I1" s="26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
@@ -4529,8 +4582,11 @@
       <c r="I2" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -4555,8 +4611,11 @@
       <c r="I3" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
@@ -4579,8 +4638,11 @@
       <c r="I4" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
@@ -4600,8 +4662,11 @@
       <c r="I5" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -4620,7 +4685,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
@@ -4639,7 +4704,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
@@ -4658,7 +4723,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
@@ -4677,7 +4742,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
@@ -4688,7 +4753,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
@@ -4696,7 +4761,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>14</v>
       </c>
@@ -4705,22 +4770,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -4751,7 +4816,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="38OCcY3c3tHtyeIpk3IqScWOh7iIMo1IG+4gNPnnbGelIJ7I6qM4m2PBaYdfDCr3D1+8d6PP10rvbad+g0LQUA==" saltValue="FZHe49NLdYkNTHLciyLA4w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nchkRp4LKzujOVPkyg+Ddfn/QXMlIToYbNo4RmKLXL5e4nTerFDssE/oozivV1JeUb4OTPlWNIYCu4M8YAH4hw==" saltValue="KYquoNmL1PCputUkzcTTPg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
finalizando sueldos comunes + SAC
</commit_message>
<xml_diff>
--- a/Woopin.SGC.Web/App_Data/Importaciones/Templates/Empleados.xlsx
+++ b/Woopin.SGC.Web/App_Data/Importaciones/Templates/Empleados.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>Dpto</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Fecha Antiguedad Reconocida</t>
+  </si>
+  <si>
+    <t>Beneficiario Obra Social</t>
   </si>
 </sst>
 </file>
@@ -900,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y576"/>
+  <dimension ref="A1:Z576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -929,10 +932,11 @@
     <col min="23" max="23" width="15.26953125" style="1" customWidth="1"/>
     <col min="24" max="24" width="15.36328125" style="1" customWidth="1"/>
     <col min="25" max="25" width="26.54296875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.90625" style="1"/>
+    <col min="26" max="26" width="23.1796875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -1008,8 +1012,11 @@
       <c r="Y1" s="21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="str">
         <f>MID(A2,4,8)</f>
@@ -1038,8 +1045,9 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z2" s="3"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="str">
         <f t="shared" ref="B3:B66" si="0">MID(A3,4,8)</f>
         <v/>
@@ -1049,7 +1057,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1059,7 +1067,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1069,7 +1077,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1079,7 +1087,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1089,7 +1097,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1099,7 +1107,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1109,7 +1117,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1119,7 +1127,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1129,7 +1137,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1139,7 +1147,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1149,7 +1157,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1159,7 +1167,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1169,7 +1177,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>